<commit_message>
adding more info to gantt
</commit_message>
<xml_diff>
--- a/gantt_chart.xlsx
+++ b/gantt_chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5fe6fa7f7cb912b1/Documents/NYU_CUSP/Spring2020/Capstone/nyconnect/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erikl\OneDrive\Documents\NYU_CUSP\Spring2020\Capstone\nyconnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{26B54AAD-4785-4DD0-B010-C2C0EF1C7278}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{FF910A6F-24A9-41A0-B772-8CB846320680}"/>
+  <xr:revisionPtr revIDLastSave="248" documentId="8_{26B54AAD-4785-4DD0-B010-C2C0EF1C7278}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{C834F869-C616-4506-8227-C54881FF3592}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{F39B1A4A-2C6C-4D57-B2D1-9AA4DED3A432}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Establish research question</t>
   </si>
@@ -111,14 +111,32 @@
     <t>First-7</t>
   </si>
   <si>
-    <t>Data Analysis/ML</t>
+    <t>Preliminary Data Analysis</t>
+  </si>
+  <si>
+    <t>Final Data Analysis/ML</t>
+  </si>
+  <si>
+    <t>Data Visualizations</t>
+  </si>
+  <si>
+    <t>Website Publishing</t>
+  </si>
+  <si>
+    <t>Set Up Hosting</t>
+  </si>
+  <si>
+    <t>Format/Publish Website</t>
+  </si>
+  <si>
+    <t>Finalize Analytics/Visualisations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,16 +152,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -151,23 +193,456 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -183,6 +658,102 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>385996</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>126692</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>386356</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>127052</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="3" name="Ink 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CD8944F-148C-426E-8591-6E0F26DEA4BD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="10725913" y="2534400"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="3" name="Ink 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CD8944F-148C-426E-8591-6E0F26DEA4BD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10717273" y="2525760"/>
+              <a:ext cx="18000" cy="18000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-03-28T02:28:51.409"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1,'0'0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -482,219 +1053,740 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C37D9ED-E487-4AB5-A100-37248C7EB813}">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="52.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" customWidth="1"/>
+    <col min="3" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="6.6328125" style="17" customWidth="1"/>
+    <col min="6" max="12" width="6.6328125" customWidth="1"/>
+    <col min="13" max="13" width="6.6328125" style="17" customWidth="1"/>
+    <col min="14" max="22" width="6.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3" t="s">
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3" t="s">
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
+      <c r="V1" s="24"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="36" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="26" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="B3" s="37">
+        <v>43898</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="43"/>
+    </row>
+    <row r="4" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="27" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="B4" s="38">
+        <v>43898</v>
+      </c>
+      <c r="C4" s="44"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="45"/>
+    </row>
+    <row r="5" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="27" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="B5" s="38">
+        <v>43898</v>
+      </c>
+      <c r="C5" s="46"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="45"/>
+    </row>
+    <row r="6" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="28" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B6" s="38">
+        <v>43905</v>
+      </c>
+      <c r="C6" s="47"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="45"/>
+    </row>
+    <row r="7" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="28" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="B7" s="38">
+        <v>43915</v>
+      </c>
+      <c r="C7" s="48"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="45"/>
+    </row>
+    <row r="8" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="27" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="B8" s="38">
+        <v>43912</v>
+      </c>
+      <c r="C8" s="48"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="45"/>
+    </row>
+    <row r="9" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="27" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B9" s="38">
+        <v>43915</v>
+      </c>
+      <c r="C9" s="48"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="45"/>
+    </row>
+    <row r="10" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="28" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B10" s="38">
+        <v>43936</v>
+      </c>
+      <c r="C10" s="48"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="45"/>
+    </row>
+    <row r="11" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="38">
         <v>43922</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="C11" s="48"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="45"/>
+    </row>
+    <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="38">
         <v>43922</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="C12" s="48"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="45"/>
+    </row>
+    <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="B13" s="38">
+        <v>43952</v>
+      </c>
+      <c r="C13" s="48"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="45"/>
+    </row>
+    <row r="14" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="38">
         <v>43957</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="C14" s="48"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="45"/>
+    </row>
+    <row r="15" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="38">
         <v>43957</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="C15" s="48"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="45"/>
+    </row>
+    <row r="16" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="38">
+        <v>44003</v>
+      </c>
+      <c r="C16" s="48"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="45"/>
+    </row>
+    <row r="17" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="38">
+        <v>44003</v>
+      </c>
+      <c r="C17" s="48"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="45"/>
+    </row>
+    <row r="18" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="38">
+        <v>44031</v>
+      </c>
+      <c r="C18" s="48"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="45"/>
+    </row>
+    <row r="19" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="38">
+        <v>44004</v>
+      </c>
+      <c r="C19" s="48"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="45"/>
+    </row>
+    <row r="20" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="38">
+        <v>44031</v>
+      </c>
+      <c r="C20" s="48"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="45"/>
+    </row>
+    <row r="21" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B21" s="38">
         <v>44004</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="C21" s="48"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="45"/>
+    </row>
+    <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="38">
+        <v>44027</v>
+      </c>
+      <c r="C22" s="48"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="45"/>
+    </row>
+    <row r="23" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B23" s="38">
         <v>44032</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="C23" s="48"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="49"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A24" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B24" s="39">
         <v>44035</v>
       </c>
+      <c r="C24" s="50"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="52"/>
+      <c r="N24" s="51"/>
+      <c r="O24" s="51"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="51"/>
+      <c r="R24" s="51"/>
+      <c r="S24" s="51"/>
+      <c r="T24" s="51"/>
+      <c r="U24" s="53"/>
+      <c r="V24" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -708,5 +1800,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>